<commit_message>
Merged Chelseas results with mines from Usability Observation notes
</commit_message>
<xml_diff>
--- a/Ibrahim_210029073_findings/data_analysis.xlsx
+++ b/Ibrahim_210029073_findings/data_analysis.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26409"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E62A88B-9EC8-4087-98A6-E7A62DC36E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="150" windowWidth="13335" windowHeight="7440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="150" windowWidth="13335" windowHeight="7440" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Overview" sheetId="1" r:id="rId1"/>
+    <sheet name="Satisfaction between Age Groups" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="43">
   <si>
     <t>Data Analysis for Usability Testing</t>
   </si>
@@ -99,13 +98,73 @@
   </si>
   <si>
     <t>Though 10% have noted that, for each session that they use the diet awareness system, it will involve them to manually set their dietary preferences, and would like to simply browse through the shop rather than spending 5 minutes or more when setting their dietary preferences.</t>
+  </si>
+  <si>
+    <t>User1</t>
+  </si>
+  <si>
+    <t>User2</t>
+  </si>
+  <si>
+    <t>Users</t>
+  </si>
+  <si>
+    <t>User3</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Test1</t>
+  </si>
+  <si>
+    <t>Test2</t>
+  </si>
+  <si>
+    <t>Test3</t>
+  </si>
+  <si>
+    <t>Test4</t>
+  </si>
+  <si>
+    <t>Test5</t>
+  </si>
+  <si>
+    <t>Users Satisfaction Level between Tests</t>
+  </si>
+  <si>
+    <t>Users 50+</t>
+  </si>
+  <si>
+    <t>TestC</t>
+  </si>
+  <si>
+    <t>TestD</t>
+  </si>
+  <si>
+    <t>TestE</t>
+  </si>
+  <si>
+    <t>TestB</t>
+  </si>
+  <si>
+    <t>TestA</t>
+  </si>
+  <si>
+    <t>Users Between 18-30</t>
+  </si>
+  <si>
+    <t>Stat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,6 +209,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -182,7 +277,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -235,13 +330,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2"/>
@@ -252,8 +367,8 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -267,16 +382,392 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
+    <cellStyle name="Heading 1" xfId="3" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="4" builtinId="17"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="32">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -292,6 +783,773 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-GB"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Users Satisfaction Level - Age 50+</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Satisfaction between Age Groups'!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Min</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Satisfaction between Age Groups'!$B$7:$F$7</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Test1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Test2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Test3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Test4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Test5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Satisfaction between Age Groups'!$B$8:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Satisfaction between Age Groups'!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Satisfaction between Age Groups'!$B$7:$F$7</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Test1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Test2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Test3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Test4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Test5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Satisfaction between Age Groups'!$B$9:$F$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Satisfaction between Age Groups'!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Max</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Satisfaction between Age Groups'!$B$7:$F$7</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Test1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Test2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Test3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Test4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Test5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Satisfaction between Age Groups'!$B$10:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:upDownBars>
+          <c:gapWidth val="150"/>
+          <c:upBars/>
+          <c:downBars/>
+        </c:upDownBars>
+        <c:marker val="1"/>
+        <c:axId val="51531776"/>
+        <c:axId val="54707328"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="51531776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Test Peformed</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="54707328"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="54707328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr" rtl="0">
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Satisfaction Level from 1 to 10</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="51531776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-GB"/>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>User Satisfaction Level - Age 18-30</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Satisfaction between Age Groups'!$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Min</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Satisfaction between Age Groups'!$B$18:$F$18</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Test1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Test2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Test3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Test4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Test5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Satisfaction between Age Groups'!$B$19:$F$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Satisfaction between Age Groups'!$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Satisfaction between Age Groups'!$B$18:$F$18</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Test1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Test2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Test3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Test4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Test5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Satisfaction between Age Groups'!$B$20:$F$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>3.3333333333333335</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.3333333333333339</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Satisfaction between Age Groups'!$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Max</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Satisfaction between Age Groups'!$B$18:$F$18</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Test1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Test2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Test3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Test4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Test5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Satisfaction between Age Groups'!$B$21:$F$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:upDownBars>
+          <c:gapWidth val="150"/>
+          <c:upBars/>
+          <c:downBars/>
+        </c:upDownBars>
+        <c:marker val="1"/>
+        <c:axId val="81226368"/>
+        <c:axId val="81241216"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="81226368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Tests Performed</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="81241216"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="81241216"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Satisfaction Level from 1 to 10</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="81226368"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="Arial" pitchFamily="34" charset="0"/>
+          <a:cs typeface="Arial" pitchFamily="34" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A7:F10" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+  <autoFilter ref="A7:F10"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Stat" dataDxfId="29"/>
+    <tableColumn id="2" name="Test1" dataDxfId="28"/>
+    <tableColumn id="3" name="Test2" dataDxfId="27"/>
+    <tableColumn id="4" name="Test3" dataDxfId="26"/>
+    <tableColumn id="5" name="Test4" dataDxfId="25"/>
+    <tableColumn id="6" name="Test5" dataDxfId="24"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:F5" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="A3:F5"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Users" dataDxfId="21"/>
+    <tableColumn id="2" name="Test1" dataDxfId="20"/>
+    <tableColumn id="3" name="Test2" dataDxfId="19"/>
+    <tableColumn id="4" name="Test3" dataDxfId="18"/>
+    <tableColumn id="5" name="Test4" dataDxfId="17"/>
+    <tableColumn id="6" name="Test5" dataDxfId="16"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A18:F21" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="A18:F21"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Stat" dataDxfId="13"/>
+    <tableColumn id="2" name="Test1" dataDxfId="12"/>
+    <tableColumn id="3" name="Test2" dataDxfId="11"/>
+    <tableColumn id="4" name="Test3" dataDxfId="10"/>
+    <tableColumn id="5" name="Test4" dataDxfId="9"/>
+    <tableColumn id="6" name="Test5" dataDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A13:F16" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="A13:F16"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Users" dataDxfId="5"/>
+    <tableColumn id="2" name="TestA" dataDxfId="4"/>
+    <tableColumn id="3" name="TestB" dataDxfId="3"/>
+    <tableColumn id="4" name="TestC" dataDxfId="2"/>
+    <tableColumn id="5" name="TestD" dataDxfId="1"/>
+    <tableColumn id="6" name="TestE" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -337,7 +1595,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -369,27 +1627,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -421,24 +1661,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -614,12 +1836,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -630,32 +1850,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15">
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
     </row>
     <row r="2" spans="2:15">
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1">
       <c r="B3" s="5" t="s">
@@ -680,14 +1900,14 @@
       <c r="O3" s="9"/>
     </row>
     <row r="4" spans="2:15">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="E4" s="11" t="s">
+      <c r="C4" s="6"/>
+      <c r="E4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="11"/>
+      <c r="F4" s="6"/>
       <c r="H4" s="10" t="s">
         <v>6</v>
       </c>
@@ -1196,16 +2416,27 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="C1:M2"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="K7:L7"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="K13:L13"/>
@@ -1222,27 +2453,16 @@
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="C1:M2"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -1250,19 +2470,422 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="20.25" thickBot="1">
+      <c r="A1" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+    </row>
+    <row r="2" spans="1:6" ht="18" thickTop="1" thickBot="1">
+      <c r="A2" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" thickTop="1">
+      <c r="A3" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="12">
+        <v>2</v>
+      </c>
+      <c r="C4" s="12">
+        <v>3</v>
+      </c>
+      <c r="D4" s="12">
+        <v>3</v>
+      </c>
+      <c r="E4" s="12">
+        <v>0</v>
+      </c>
+      <c r="F4" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="12">
+        <v>3.5</v>
+      </c>
+      <c r="C5" s="12">
+        <v>3</v>
+      </c>
+      <c r="D5" s="12">
+        <v>4</v>
+      </c>
+      <c r="E5" s="12">
+        <v>2</v>
+      </c>
+      <c r="F5" s="12">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="12">
+        <f>MIN(B4:B5)</f>
+        <v>2</v>
+      </c>
+      <c r="C8" s="12">
+        <f t="shared" ref="C8:F8" si="0">MIN(C4:C5)</f>
+        <v>3</v>
+      </c>
+      <c r="D8" s="12">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E8" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="12">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="12">
+        <f>AVERAGE(B4:B5)</f>
+        <v>2.75</v>
+      </c>
+      <c r="C9" s="12">
+        <f>AVERAGE(C4:C5)</f>
+        <v>3</v>
+      </c>
+      <c r="D9" s="12">
+        <f>AVERAGE(D4:D5)</f>
+        <v>3.5</v>
+      </c>
+      <c r="E9" s="12">
+        <f>AVERAGE(E4:E5)</f>
+        <v>1</v>
+      </c>
+      <c r="F9" s="12">
+        <f>AVERAGE(F4:F5)</f>
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="12">
+        <f>MAX(B4:B5)</f>
+        <v>3.5</v>
+      </c>
+      <c r="C10" s="12">
+        <f t="shared" ref="C10:F10" si="1">MAX(C4:C5)</f>
+        <v>3</v>
+      </c>
+      <c r="D10" s="12">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E10" s="12">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="F10" s="12">
+        <f t="shared" si="1"/>
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+    </row>
+    <row r="12" spans="1:6" ht="17.25" thickBot="1">
+      <c r="A12" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" thickTop="1">
+      <c r="A13" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="12">
+        <v>6</v>
+      </c>
+      <c r="C14" s="12">
+        <v>4</v>
+      </c>
+      <c r="D14" s="12">
+        <v>6</v>
+      </c>
+      <c r="E14" s="12">
+        <v>10</v>
+      </c>
+      <c r="F14" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="12">
+        <v>0</v>
+      </c>
+      <c r="C15" s="12">
+        <v>6</v>
+      </c>
+      <c r="D15" s="12">
+        <v>5</v>
+      </c>
+      <c r="E15" s="12">
+        <v>8</v>
+      </c>
+      <c r="F15" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="12">
+        <v>4</v>
+      </c>
+      <c r="C16" s="12">
+        <v>5</v>
+      </c>
+      <c r="D16" s="12">
+        <v>4</v>
+      </c>
+      <c r="E16" s="12">
+        <v>10</v>
+      </c>
+      <c r="F16" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="12">
+        <f>MIN(B14:B16)</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="12">
+        <f t="shared" ref="C19:F19" si="2">MIN(C14:C16)</f>
+        <v>4</v>
+      </c>
+      <c r="D19" s="12">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E19" s="12">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="F19" s="12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="12">
+        <f>AVERAGE(B14:B16)</f>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="C20" s="12">
+        <f>AVERAGE(C14:C16)</f>
+        <v>5</v>
+      </c>
+      <c r="D20" s="12">
+        <f>AVERAGE(D14:D16)</f>
+        <v>5</v>
+      </c>
+      <c r="E20" s="12">
+        <f>AVERAGE(E14:E16)</f>
+        <v>9.3333333333333339</v>
+      </c>
+      <c r="F20" s="12">
+        <f>AVERAGE(F14:F16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="12">
+        <f>MAX(B14:B16)</f>
+        <v>6</v>
+      </c>
+      <c r="C21" s="12">
+        <f t="shared" ref="C21:F21" si="3">MAX(C14:C16)</f>
+        <v>6</v>
+      </c>
+      <c r="D21" s="12">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="E21" s="12">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="F21" s="12">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A2:F2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="4">
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated Graph according to some emissions from result
</commit_message>
<xml_diff>
--- a/Ibrahim_210029073_findings/data_analysis.xlsx
+++ b/Ibrahim_210029073_findings/data_analysis.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="38">
   <si>
     <t>Data Analysis for Usability Testing</t>
   </si>
@@ -137,21 +137,6 @@
   </si>
   <si>
     <t>Users 50+</t>
-  </si>
-  <si>
-    <t>TestC</t>
-  </si>
-  <si>
-    <t>TestD</t>
-  </si>
-  <si>
-    <t>TestE</t>
-  </si>
-  <si>
-    <t>TestB</t>
-  </si>
-  <si>
-    <t>TestA</t>
   </si>
   <si>
     <t>Users Between 18-30</t>
@@ -810,7 +795,7 @@
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
-        <c:grouping val="stacked"/>
+        <c:grouping val="standard"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1126,7 +1111,7 @@
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
-        <c:grouping val="stacked"/>
+        <c:grouping val="standard"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
@@ -1176,7 +1161,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>4</c:v>
@@ -1185,10 +1170,10 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>8</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1243,7 +1228,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>3.3333333333333335</c:v>
+                  <c:v>6.666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>5</c:v>
@@ -1252,10 +1237,10 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.3333333333333339</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1310,7 +1295,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>6</c:v>
@@ -1319,10 +1304,10 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1542,11 +1527,11 @@
   <autoFilter ref="A13:F16"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Users" dataDxfId="5"/>
-    <tableColumn id="2" name="TestA" dataDxfId="4"/>
-    <tableColumn id="3" name="TestB" dataDxfId="3"/>
-    <tableColumn id="4" name="TestC" dataDxfId="2"/>
-    <tableColumn id="5" name="TestD" dataDxfId="1"/>
-    <tableColumn id="6" name="TestE" dataDxfId="0"/>
+    <tableColumn id="2" name="Test1" dataDxfId="4"/>
+    <tableColumn id="3" name="Test2" dataDxfId="3"/>
+    <tableColumn id="4" name="Test3" dataDxfId="2"/>
+    <tableColumn id="5" name="Test4" dataDxfId="1"/>
+    <tableColumn id="6" name="Test5" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2474,7 +2459,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2572,7 +2557,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="12" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>29</v>
@@ -2675,7 +2660,7 @@
     </row>
     <row r="12" spans="1:6" ht="17.25" thickBot="1">
       <c r="A12" s="14" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
@@ -2688,19 +2673,19 @@
         <v>25</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -2708,19 +2693,19 @@
         <v>23</v>
       </c>
       <c r="B14" s="12">
+        <v>4</v>
+      </c>
+      <c r="C14" s="12">
         <v>6</v>
       </c>
-      <c r="C14" s="12">
+      <c r="D14" s="12">
         <v>4</v>
       </c>
-      <c r="D14" s="12">
-        <v>6</v>
-      </c>
       <c r="E14" s="12">
+        <v>0</v>
+      </c>
+      <c r="F14" s="12">
         <v>10</v>
-      </c>
-      <c r="F14" s="12">
-        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -2728,19 +2713,19 @@
         <v>24</v>
       </c>
       <c r="B15" s="12">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C15" s="12">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D15" s="12">
         <v>5</v>
       </c>
       <c r="E15" s="12">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F15" s="12">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -2748,19 +2733,19 @@
         <v>26</v>
       </c>
       <c r="B16" s="12">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C16" s="12">
         <v>5</v>
       </c>
       <c r="D16" s="12">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E16" s="12">
+        <v>0</v>
+      </c>
+      <c r="F16" s="12">
         <v>10</v>
-      </c>
-      <c r="F16" s="12">
-        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -2773,7 +2758,7 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="12" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>29</v>
@@ -2797,7 +2782,7 @@
       </c>
       <c r="B19" s="12">
         <f>MIN(B14:B16)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="C19" s="12">
         <f t="shared" ref="C19:F19" si="2">MIN(C14:C16)</f>
@@ -2809,11 +2794,11 @@
       </c>
       <c r="E19" s="12">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F19" s="12">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -2822,7 +2807,7 @@
       </c>
       <c r="B20" s="12">
         <f>AVERAGE(B14:B16)</f>
-        <v>3.3333333333333335</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="C20" s="12">
         <f>AVERAGE(C14:C16)</f>
@@ -2834,11 +2819,11 @@
       </c>
       <c r="E20" s="12">
         <f>AVERAGE(E14:E16)</f>
-        <v>9.3333333333333339</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="F20" s="12">
         <f>AVERAGE(F14:F16)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -2847,7 +2832,7 @@
       </c>
       <c r="B21" s="12">
         <f>MAX(B14:B16)</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C21" s="12">
         <f t="shared" ref="C21:F21" si="3">MAX(C14:C16)</f>
@@ -2859,11 +2844,11 @@
       </c>
       <c r="E21" s="12">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F21" s="12">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Graph by applying standard deviation
</commit_message>
<xml_diff>
--- a/Ibrahim_210029073_findings/data_analysis.xlsx
+++ b/Ibrahim_210029073_findings/data_analysis.xlsx
@@ -815,6 +815,12 @@
             <c:errBarType val="both"/>
             <c:errValType val="stdErr"/>
           </c:errBars>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="fixedVal"/>
+            <c:val val="1"/>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>'Satisfaction between Age Groups'!$B$7:$F$7</c:f>
@@ -877,6 +883,12 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdDev"/>
+            <c:val val="1"/>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>'Satisfaction between Age Groups'!$B$7:$F$7</c:f>
@@ -939,6 +951,13 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="minus"/>
+            <c:errValType val="fixedVal"/>
+            <c:noEndCap val="1"/>
+            <c:val val="1"/>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>'Satisfaction between Age Groups'!$B$7:$F$7</c:f>
@@ -1129,7 +1148,8 @@
           <c:errBars>
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
+            <c:errValType val="stdDev"/>
+            <c:val val="1"/>
           </c:errBars>
           <c:cat>
             <c:strRef>
@@ -1196,7 +1216,8 @@
           <c:errBars>
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
+            <c:errValType val="stdDev"/>
+            <c:val val="1"/>
           </c:errBars>
           <c:cat>
             <c:strRef>
@@ -1263,7 +1284,8 @@
           <c:errBars>
             <c:errDir val="y"/>
             <c:errBarType val="both"/>
-            <c:errValType val="stdErr"/>
+            <c:errValType val="stdDev"/>
+            <c:val val="1"/>
           </c:errBars>
           <c:cat>
             <c:strRef>
@@ -2459,7 +2481,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="R27" sqref="R27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Updated box plot diagram
</commit_message>
<xml_diff>
--- a/Ibrahim_210029073_findings/data_analysis.xlsx
+++ b/Ibrahim_210029073_findings/data_analysis.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -384,11 +383,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -402,17 +404,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="4" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1230,11 +1229,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="60673408"/>
-        <c:axId val="60822272"/>
+        <c:axId val="109512192"/>
+        <c:axId val="109522944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="60673408"/>
+        <c:axId val="109512192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1263,14 +1262,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60822272"/>
+        <c:crossAx val="109522944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="60822272"/>
+        <c:axId val="109522944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1296,7 +1295,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="60673408"/>
+        <c:crossAx val="109512192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1321,7 +1320,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1371,6 +1370,11 @@
           <c:spPr>
             <a:noFill/>
           </c:spPr>
+          <c:errBars>
+            <c:errBarType val="minus"/>
+            <c:errValType val="percentage"/>
+            <c:val val="100"/>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>'Satisfaction between Age Groups'!$B$30:$F$30</c:f>
@@ -1619,6 +1623,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:errBars>
+            <c:errBarType val="plus"/>
+            <c:errValType val="percentage"/>
+            <c:val val="100"/>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>'Satisfaction between Age Groups'!$B$30:$F$30</c:f>
@@ -1668,11 +1677,11 @@
           </c:val>
         </c:ser>
         <c:overlap val="100"/>
-        <c:axId val="63021440"/>
-        <c:axId val="63022976"/>
+        <c:axId val="109972480"/>
+        <c:axId val="109991040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="63021440"/>
+        <c:axId val="109972480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1696,14 +1705,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63022976"/>
+        <c:crossAx val="109991040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="63022976"/>
+        <c:axId val="109991040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1729,7 +1738,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="63021440"/>
+        <c:crossAx val="109972480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1754,7 +1763,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2195,142 +2204,142 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15">
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
     </row>
     <row r="2" spans="2:15">
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7"/>
-      <c r="M2" s="7"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="E3" s="6" t="s">
+      <c r="C3" s="7"/>
+      <c r="E3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="H3" s="10" t="s">
+      <c r="F3" s="7"/>
+      <c r="H3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="10"/>
-      <c r="K3" s="10" t="s">
+      <c r="I3" s="11"/>
+      <c r="K3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="10"/>
-      <c r="N3" s="10" t="s">
+      <c r="L3" s="11"/>
+      <c r="N3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="10"/>
+      <c r="O3" s="11"/>
     </row>
     <row r="4" spans="2:15">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="E4" s="12" t="s">
+      <c r="C4" s="8"/>
+      <c r="E4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="12"/>
-      <c r="H4" s="11" t="s">
+      <c r="F4" s="8"/>
+      <c r="H4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="11"/>
-      <c r="K4" s="11" t="s">
+      <c r="I4" s="12"/>
+      <c r="K4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="11"/>
-      <c r="N4" s="11" t="s">
+      <c r="L4" s="12"/>
+      <c r="N4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="O4" s="11"/>
+      <c r="O4" s="12"/>
     </row>
     <row r="5" spans="2:15">
-      <c r="B5" s="9">
+      <c r="B5" s="10">
         <v>4</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="E5" s="9">
+      <c r="C5" s="10"/>
+      <c r="E5" s="10">
         <v>2</v>
       </c>
-      <c r="F5" s="9"/>
-      <c r="H5" s="9">
+      <c r="F5" s="10"/>
+      <c r="H5" s="10">
         <v>4</v>
       </c>
-      <c r="I5" s="9"/>
-      <c r="K5" s="9">
+      <c r="I5" s="10"/>
+      <c r="K5" s="10">
         <v>6</v>
       </c>
-      <c r="L5" s="9"/>
-      <c r="N5" s="9">
+      <c r="L5" s="10"/>
+      <c r="N5" s="10">
         <v>0</v>
       </c>
-      <c r="O5" s="9"/>
+      <c r="O5" s="10"/>
     </row>
     <row r="6" spans="2:15">
-      <c r="B6" s="9">
+      <c r="B6" s="10">
         <v>2</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="E6" s="9">
+      <c r="C6" s="10"/>
+      <c r="E6" s="10">
         <v>0</v>
       </c>
-      <c r="F6" s="9"/>
-      <c r="H6" s="9">
+      <c r="F6" s="10"/>
+      <c r="H6" s="10">
         <v>6</v>
       </c>
-      <c r="I6" s="9"/>
-      <c r="K6" s="9">
+      <c r="I6" s="10"/>
+      <c r="K6" s="10">
         <v>10</v>
       </c>
-      <c r="L6" s="9"/>
-      <c r="N6" s="9">
+      <c r="L6" s="10"/>
+      <c r="N6" s="10">
         <v>3</v>
       </c>
-      <c r="O6" s="9"/>
+      <c r="O6" s="10"/>
     </row>
     <row r="7" spans="2:15">
-      <c r="B7" s="9">
+      <c r="B7" s="10">
         <v>2</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="E7" s="9">
+      <c r="C7" s="10"/>
+      <c r="E7" s="10">
         <v>2</v>
       </c>
-      <c r="F7" s="9"/>
-      <c r="H7" s="9">
+      <c r="F7" s="10"/>
+      <c r="H7" s="10">
         <v>8</v>
       </c>
-      <c r="I7" s="9"/>
-      <c r="K7" s="9">
+      <c r="I7" s="10"/>
+      <c r="K7" s="10">
         <v>8</v>
       </c>
-      <c r="L7" s="9"/>
-      <c r="N7" s="9">
+      <c r="L7" s="10"/>
+      <c r="N7" s="10">
         <v>0</v>
       </c>
-      <c r="O7" s="9"/>
+      <c r="O7" s="10"/>
     </row>
     <row r="8" spans="2:15">
       <c r="B8" s="1" t="s">
@@ -2481,92 +2490,92 @@
       </c>
     </row>
     <row r="13" spans="2:15">
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="E13" s="8" t="s">
+      <c r="C13" s="9"/>
+      <c r="E13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="8"/>
-      <c r="H13" s="8" t="s">
+      <c r="F13" s="9"/>
+      <c r="H13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I13" s="8"/>
-      <c r="K13" s="8" t="s">
+      <c r="I13" s="9"/>
+      <c r="K13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="L13" s="8"/>
-      <c r="N13" s="8" t="s">
+      <c r="L13" s="9"/>
+      <c r="N13" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="O13" s="8"/>
+      <c r="O13" s="9"/>
     </row>
     <row r="14" spans="2:15">
-      <c r="B14" s="9">
+      <c r="B14" s="10">
         <v>6</v>
       </c>
-      <c r="C14" s="9"/>
-      <c r="E14" s="9">
+      <c r="C14" s="10"/>
+      <c r="E14" s="10">
         <v>4</v>
       </c>
-      <c r="F14" s="9"/>
-      <c r="H14" s="9">
+      <c r="F14" s="10"/>
+      <c r="H14" s="10">
         <v>6</v>
       </c>
-      <c r="I14" s="9"/>
-      <c r="K14" s="9">
+      <c r="I14" s="10"/>
+      <c r="K14" s="10">
         <v>10</v>
       </c>
-      <c r="L14" s="9"/>
-      <c r="N14" s="9">
+      <c r="L14" s="10"/>
+      <c r="N14" s="10">
         <v>0</v>
       </c>
-      <c r="O14" s="9"/>
+      <c r="O14" s="10"/>
     </row>
     <row r="15" spans="2:15">
-      <c r="B15" s="9">
+      <c r="B15" s="10">
         <v>0</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="E15" s="9">
+      <c r="C15" s="10"/>
+      <c r="E15" s="10">
         <v>6</v>
       </c>
-      <c r="F15" s="9"/>
-      <c r="H15" s="9">
+      <c r="F15" s="10"/>
+      <c r="H15" s="10">
         <v>5</v>
       </c>
-      <c r="I15" s="9"/>
-      <c r="K15" s="9">
+      <c r="I15" s="10"/>
+      <c r="K15" s="10">
         <v>8</v>
       </c>
-      <c r="L15" s="9"/>
-      <c r="N15" s="9">
+      <c r="L15" s="10"/>
+      <c r="N15" s="10">
         <v>0</v>
       </c>
-      <c r="O15" s="9"/>
+      <c r="O15" s="10"/>
     </row>
     <row r="16" spans="2:15">
-      <c r="B16" s="9">
+      <c r="B16" s="10">
         <v>4</v>
       </c>
-      <c r="C16" s="9"/>
-      <c r="E16" s="9">
+      <c r="C16" s="10"/>
+      <c r="E16" s="10">
         <v>5</v>
       </c>
-      <c r="F16" s="9"/>
-      <c r="H16" s="9">
+      <c r="F16" s="10"/>
+      <c r="H16" s="10">
         <v>4</v>
       </c>
-      <c r="I16" s="9"/>
-      <c r="K16" s="9">
+      <c r="I16" s="10"/>
+      <c r="K16" s="10">
         <v>10</v>
       </c>
-      <c r="L16" s="9"/>
-      <c r="N16" s="9">
+      <c r="L16" s="10"/>
+      <c r="N16" s="10">
         <v>0</v>
       </c>
-      <c r="O16" s="9"/>
+      <c r="O16" s="10"/>
     </row>
     <row r="17" spans="2:15">
       <c r="B17" s="1" t="s">
@@ -2717,13 +2726,13 @@
       </c>
     </row>
     <row r="22" spans="2:15">
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
     </row>
     <row r="23" spans="2:15" ht="270" customHeight="1">
       <c r="B23" s="4" t="s">
@@ -2761,16 +2770,27 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="C1:M2"/>
+    <mergeCell ref="N13:O13"/>
+    <mergeCell ref="N14:O14"/>
+    <mergeCell ref="N15:O15"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="N3:O3"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="N7:O7"/>
+    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="H14:I14"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="K7:L7"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="K13:L13"/>
@@ -2787,27 +2807,16 @@
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="H6:I6"/>
     <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H14:I14"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="K14:L14"/>
-    <mergeCell ref="K7:L7"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="C1:M2"/>
-    <mergeCell ref="N13:O13"/>
-    <mergeCell ref="N14:O14"/>
-    <mergeCell ref="N15:O15"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="K5:L5"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="N3:O3"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="N7:O7"/>
-    <mergeCell ref="H15:I15"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="B5:C5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2818,8 +2827,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
+      <selection activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -2831,24 +2840,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" thickBot="1">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" ht="18" thickTop="1" thickBot="1">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
     </row>
     <row r="3" spans="1:6" ht="15" thickTop="1">
       <c r="A3" s="5" t="s">
@@ -3006,14 +3015,14 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="17.25" thickBot="1">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
     </row>
     <row r="13" spans="1:6" ht="15" thickTop="1">
       <c r="A13" s="5" t="s">
@@ -3270,19 +3279,19 @@
       <c r="A30" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D30" s="15" t="s">
+      <c r="D30" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E30" s="15" t="s">
+      <c r="E30" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F30" s="15" t="s">
+      <c r="F30" s="6" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3415,19 +3424,19 @@
       <c r="A37" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="B37" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C37" s="15" t="s">
+      <c r="C37" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D37" s="15" t="s">
+      <c r="D37" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E37" s="15" t="s">
+      <c r="E37" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="F37" s="15" t="s">
+      <c r="F37" s="6" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
data_analysis.xlsx | Updated stat information in Overview sheet
</commit_message>
<xml_diff>
--- a/Ibrahim_210029073_findings/data_analysis.xlsx
+++ b/Ibrahim_210029073_findings/data_analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="150" windowWidth="13335" windowHeight="7440" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="150" windowWidth="13335" windowHeight="7440"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -421,7 +421,281 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Output" xfId="1" builtinId="21"/>
   </cellStyles>
-  <dxfs count="37">
+  <dxfs count="53">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -932,6 +1206,14 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:noFill/>
+          </c:spPr>
+          <c:errBars>
+            <c:errBarType val="minus"/>
+            <c:errValType val="percentage"/>
+            <c:val val="50"/>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>'Satisfaction between Age Groups'!$B$37:$F$37</c:f>
@@ -1180,6 +1462,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:errBars>
+            <c:errBarType val="plus"/>
+            <c:errValType val="percentage"/>
+            <c:val val="50"/>
+          </c:errBars>
           <c:cat>
             <c:strRef>
               <c:f>'Satisfaction between Age Groups'!$B$37:$F$37</c:f>
@@ -1373,7 +1660,7 @@
           <c:errBars>
             <c:errBarType val="minus"/>
             <c:errValType val="percentage"/>
-            <c:val val="100"/>
+            <c:val val="50"/>
           </c:errBars>
           <c:cat>
             <c:strRef>
@@ -1626,7 +1913,7 @@
           <c:errBars>
             <c:errBarType val="plus"/>
             <c:errValType val="percentage"/>
-            <c:val val="100"/>
+            <c:val val="50"/>
           </c:errBars>
           <c:cat>
             <c:strRef>
@@ -1835,8 +2122,38 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A7:F10" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A7:F10" totalsRowShown="0" headerRowDxfId="52" dataDxfId="51">
   <autoFilter ref="A7:F10"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Stat" dataDxfId="50"/>
+    <tableColumn id="2" name="Test1" dataDxfId="49"/>
+    <tableColumn id="3" name="Test2" dataDxfId="48"/>
+    <tableColumn id="4" name="Test3" dataDxfId="47"/>
+    <tableColumn id="5" name="Test4" dataDxfId="46"/>
+    <tableColumn id="6" name="Test5" dataDxfId="45"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:F5" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43">
+  <autoFilter ref="A3:F5"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Users" dataDxfId="42"/>
+    <tableColumn id="2" name="Test1" dataDxfId="41"/>
+    <tableColumn id="3" name="Test2" dataDxfId="40"/>
+    <tableColumn id="4" name="Test3" dataDxfId="39"/>
+    <tableColumn id="5" name="Test4" dataDxfId="38"/>
+    <tableColumn id="6" name="Test5" dataDxfId="37"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A18:F21" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
+  <autoFilter ref="A18:F21"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Stat" dataDxfId="34"/>
     <tableColumn id="2" name="Test1" dataDxfId="33"/>
@@ -1849,9 +2166,9 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A3:F5" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
-  <autoFilter ref="A3:F5"/>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A13:F16" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+  <autoFilter ref="A13:F16"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Users" dataDxfId="26"/>
     <tableColumn id="2" name="Test1" dataDxfId="25"/>
@@ -1864,43 +2181,43 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A18:F21" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
-  <autoFilter ref="A18:F21"/>
-  <tableColumns count="6">
-    <tableColumn id="1" name="Stat" dataDxfId="18"/>
-    <tableColumn id="2" name="Test1" dataDxfId="17"/>
-    <tableColumn id="3" name="Test2" dataDxfId="16"/>
-    <tableColumn id="4" name="Test3" dataDxfId="15"/>
-    <tableColumn id="5" name="Test4" dataDxfId="14"/>
-    <tableColumn id="6" name="Test5" dataDxfId="13"/>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A23:C28" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+  <autoFilter ref="A23:C28"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Test" dataDxfId="18"/>
+    <tableColumn id="2" name="Average 18-30" dataDxfId="17"/>
+    <tableColumn id="3" name="Average 50+" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A13:F16" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A13:F16"/>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A30:F35" totalsRowShown="0" headerRowDxfId="8" dataDxfId="9">
+  <autoFilter ref="A30:F35"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Users" dataDxfId="10"/>
-    <tableColumn id="2" name="Test1" dataDxfId="9"/>
-    <tableColumn id="3" name="Test2" dataDxfId="8"/>
-    <tableColumn id="4" name="Test3" dataDxfId="7"/>
-    <tableColumn id="5" name="Test4" dataDxfId="6"/>
-    <tableColumn id="6" name="Test5" dataDxfId="5"/>
+    <tableColumn id="1" name="Stat" dataDxfId="15"/>
+    <tableColumn id="2" name="Browse Products" dataDxfId="14"/>
+    <tableColumn id="3" name="Add Item to Basket" dataDxfId="13"/>
+    <tableColumn id="4" name="View Recommended Products" dataDxfId="12"/>
+    <tableColumn id="5" name="Visit Dietary Features" dataDxfId="11"/>
+    <tableColumn id="6" name="Set Preferences from Settings" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A23:C28" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A23:C28"/>
-  <tableColumns count="3">
-    <tableColumn id="1" name="Test" dataDxfId="2"/>
-    <tableColumn id="2" name="Average 18-30" dataDxfId="1"/>
-    <tableColumn id="3" name="Average 50+" dataDxfId="0"/>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="A37:F42" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A37:F42"/>
+  <tableColumns count="6">
+    <tableColumn id="1" name="Stat" dataDxfId="7"/>
+    <tableColumn id="2" name="Browse Products" dataDxfId="6"/>
+    <tableColumn id="3" name="Add Item to Basket" dataDxfId="5"/>
+    <tableColumn id="4" name="View Recommended Products" dataDxfId="4"/>
+    <tableColumn id="5" name="Visit Dietary Features" dataDxfId="3"/>
+    <tableColumn id="6" name="Set Preferences from Settings" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2193,7 +2510,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:O24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -2551,7 +2870,7 @@
       </c>
       <c r="L15" s="10"/>
       <c r="N15" s="10">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O15" s="10"/>
     </row>
@@ -2573,7 +2892,7 @@
       </c>
       <c r="L16" s="10"/>
       <c r="N16" s="10">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="O16" s="10"/>
     </row>
@@ -2648,7 +2967,7 @@
       </c>
       <c r="O18" s="2">
         <f>SUM(N14:N16)</f>
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="2:15">
@@ -2685,7 +3004,7 @@
       </c>
       <c r="O19" s="2">
         <f>O18/O17</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="2:15">
@@ -2722,7 +3041,7 @@
       </c>
       <c r="O20" s="3">
         <f>ROUND(O19,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="2:15">
@@ -2827,16 +3146,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" workbookViewId="0">
-      <selection activeCell="S24" sqref="S24"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26:D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" style="5" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" style="5" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="5"/>
+    <col min="2" max="2" width="19.28515625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" style="5" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="23" style="5" customWidth="1"/>
+    <col min="6" max="6" width="31.28515625" style="5" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" thickBot="1">
@@ -3549,12 +3871,14 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="5">
+  <tableParts count="7">
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
     <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
data_analysis.xlsx | updated sheet name in spreadsheet
</commit_message>
<xml_diff>
--- a/Ibrahim_210029073_findings/data_analysis.xlsx
+++ b/Ibrahim_210029073_findings/data_analysis.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26502"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="48" documentId="11_3B9EF4882D1E01A6376352BBECB9D91053EAE96E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{61586F46-A36F-44E1-8E53-D3116791720D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8887162-F9CA-4DA1-A2C4-838D1E542E66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
-    <sheet name="Satisfaction between Age Groups" sheetId="2" r:id="rId2"/>
+    <sheet name="Performance between Age Groups" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028" iterateDelta="1E-4"/>
@@ -392,33 +392,6 @@
   </cellStyleXfs>
   <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="4" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="3" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="2" applyProtection="1"/>
@@ -428,6 +401,33 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="4" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="3" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -574,7 +574,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Satisfaction between Age Groups'!$A$45</c:f>
+              <c:f>'Performance between Age Groups'!$A$45</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -641,7 +641,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>'Satisfaction between Age Groups'!$B$44:$F$44</c:f>
+              <c:f>'Performance between Age Groups'!$B$44:$F$44</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -664,7 +664,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Satisfaction between Age Groups'!$B$45:$F$45</c:f>
+              <c:f>'Performance between Age Groups'!$B$45:$F$45</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -697,7 +697,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Satisfaction between Age Groups'!$A$46</c:f>
+              <c:f>'Performance between Age Groups'!$A$46</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -752,7 +752,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Satisfaction between Age Groups'!$B$44:$F$44</c:f>
+              <c:f>'Performance between Age Groups'!$B$44:$F$44</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -775,7 +775,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Satisfaction between Age Groups'!$B$46:$F$46</c:f>
+              <c:f>'Performance between Age Groups'!$B$46:$F$46</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -808,7 +808,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Satisfaction between Age Groups'!$A$47</c:f>
+              <c:f>'Performance between Age Groups'!$A$47</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -863,7 +863,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Satisfaction between Age Groups'!$B$44:$F$44</c:f>
+              <c:f>'Performance between Age Groups'!$B$44:$F$44</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -886,7 +886,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Satisfaction between Age Groups'!$B$47:$F$47</c:f>
+              <c:f>'Performance between Age Groups'!$B$47:$F$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -919,7 +919,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Satisfaction between Age Groups'!$A$48</c:f>
+              <c:f>'Performance between Age Groups'!$A$48</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -987,7 +987,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>'Satisfaction between Age Groups'!$B$44:$F$44</c:f>
+              <c:f>'Performance between Age Groups'!$B$44:$F$44</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1010,7 +1010,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Satisfaction between Age Groups'!$B$48:$F$48</c:f>
+              <c:f>'Performance between Age Groups'!$B$48:$F$48</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1043,7 +1043,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Satisfaction between Age Groups'!$A$49</c:f>
+              <c:f>'Performance between Age Groups'!$A$49</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1096,7 +1096,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Satisfaction between Age Groups'!$B$44:$F$44</c:f>
+              <c:f>'Performance between Age Groups'!$B$44:$F$44</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1119,7 +1119,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Satisfaction between Age Groups'!$B$49:$F$49</c:f>
+              <c:f>'Performance between Age Groups'!$B$49:$F$49</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1400,7 +1400,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Satisfaction between Age Groups'!$A$37</c:f>
+              <c:f>'Performance between Age Groups'!$A$37</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1467,7 +1467,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>'Satisfaction between Age Groups'!$B$36:$F$36</c:f>
+              <c:f>'Performance between Age Groups'!$B$36:$F$36</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1490,7 +1490,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Satisfaction between Age Groups'!$B$37:$F$37</c:f>
+              <c:f>'Performance between Age Groups'!$B$37:$F$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1523,7 +1523,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Satisfaction between Age Groups'!$A$38</c:f>
+              <c:f>'Performance between Age Groups'!$A$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1578,7 +1578,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Satisfaction between Age Groups'!$B$36:$F$36</c:f>
+              <c:f>'Performance between Age Groups'!$B$36:$F$36</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1601,7 +1601,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Satisfaction between Age Groups'!$B$38:$F$38</c:f>
+              <c:f>'Performance between Age Groups'!$B$38:$F$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1634,7 +1634,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Satisfaction between Age Groups'!$A$39</c:f>
+              <c:f>'Performance between Age Groups'!$A$39</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1689,7 +1689,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Satisfaction between Age Groups'!$B$36:$F$36</c:f>
+              <c:f>'Performance between Age Groups'!$B$36:$F$36</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1712,7 +1712,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Satisfaction between Age Groups'!$B$39:$F$39</c:f>
+              <c:f>'Performance between Age Groups'!$B$39:$F$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1745,7 +1745,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Satisfaction between Age Groups'!$A$40</c:f>
+              <c:f>'Performance between Age Groups'!$A$40</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1813,7 +1813,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>'Satisfaction between Age Groups'!$B$36:$F$36</c:f>
+              <c:f>'Performance between Age Groups'!$B$36:$F$36</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -1836,7 +1836,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Satisfaction between Age Groups'!$B$40:$F$40</c:f>
+              <c:f>'Performance between Age Groups'!$B$40:$F$40</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -1869,7 +1869,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Satisfaction between Age Groups'!$A$41</c:f>
+              <c:f>'Performance between Age Groups'!$A$41</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1929,6 +1929,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-C6F3-467B-9208-8EE95543E035}"/>
                 </c:ext>
@@ -1957,6 +1958,7 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="1"/>
               <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000007-C6F3-467B-9208-8EE95543E035}"/>
                 </c:ext>
@@ -1998,7 +2000,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Satisfaction between Age Groups'!$B$36:$F$36</c:f>
+              <c:f>'Performance between Age Groups'!$B$36:$F$36</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -2021,7 +2023,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Satisfaction between Age Groups'!$B$41:$F$41</c:f>
+              <c:f>'Performance between Age Groups'!$B$41:$F$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2253,16 +2255,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>142920</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>76320</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>504870</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>142995</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>56520</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>9090</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>418470</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>132915</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2289,16 +2291,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>76320</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>123840</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>438270</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>66690</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>18360</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>8910</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>380310</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>104160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2743,32 +2745,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:15">
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
     </row>
     <row r="2" spans="2:15">
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
-      <c r="J2" s="9"/>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
     </row>
     <row r="3" spans="2:15" ht="15" customHeight="1">
       <c r="B3" s="8" t="s">
@@ -2779,487 +2781,487 @@
         <v>2</v>
       </c>
       <c r="F3" s="8"/>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="7"/>
-      <c r="K3" s="7" t="s">
+      <c r="I3" s="9"/>
+      <c r="K3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="7"/>
-      <c r="N3" s="7" t="s">
+      <c r="L3" s="9"/>
+      <c r="N3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="7"/>
+      <c r="O3" s="9"/>
     </row>
     <row r="4" spans="2:15">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="E4" s="6" t="s">
+      <c r="C4" s="10"/>
+      <c r="E4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="H4" s="5" t="s">
+      <c r="F4" s="10"/>
+      <c r="H4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="5"/>
-      <c r="K4" s="5" t="s">
+      <c r="I4" s="11"/>
+      <c r="K4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="L4" s="5"/>
-      <c r="N4" s="5" t="s">
+      <c r="L4" s="11"/>
+      <c r="N4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="O4" s="5"/>
+      <c r="O4" s="11"/>
     </row>
     <row r="5" spans="2:15">
-      <c r="B5" s="4">
+      <c r="B5" s="12">
         <v>4</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="E5" s="4">
+      <c r="C5" s="12"/>
+      <c r="E5" s="12">
         <v>2</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="H5" s="4">
+      <c r="F5" s="12"/>
+      <c r="H5" s="12">
         <v>4</v>
       </c>
-      <c r="I5" s="4"/>
-      <c r="K5" s="4">
+      <c r="I5" s="12"/>
+      <c r="K5" s="12">
         <v>6</v>
       </c>
-      <c r="L5" s="4"/>
-      <c r="N5" s="4">
+      <c r="L5" s="12"/>
+      <c r="N5" s="12">
         <v>0</v>
       </c>
-      <c r="O5" s="4"/>
+      <c r="O5" s="12"/>
     </row>
     <row r="6" spans="2:15">
-      <c r="B6" s="4">
+      <c r="B6" s="12">
         <v>2</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="E6" s="4">
+      <c r="C6" s="12"/>
+      <c r="E6" s="12">
         <v>0</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="H6" s="4">
+      <c r="F6" s="12"/>
+      <c r="H6" s="12">
         <v>6</v>
       </c>
-      <c r="I6" s="4"/>
-      <c r="K6" s="4">
+      <c r="I6" s="12"/>
+      <c r="K6" s="12">
         <v>10</v>
       </c>
-      <c r="L6" s="4"/>
-      <c r="N6" s="4">
+      <c r="L6" s="12"/>
+      <c r="N6" s="12">
         <v>3</v>
       </c>
-      <c r="O6" s="4"/>
+      <c r="O6" s="12"/>
     </row>
     <row r="7" spans="2:15">
-      <c r="B7" s="4">
+      <c r="B7" s="12">
         <v>2</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="E7" s="4">
+      <c r="C7" s="12"/>
+      <c r="E7" s="12">
         <v>2</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="H7" s="4">
+      <c r="F7" s="12"/>
+      <c r="H7" s="12">
         <v>8</v>
       </c>
-      <c r="I7" s="4"/>
-      <c r="K7" s="4">
+      <c r="I7" s="12"/>
+      <c r="K7" s="12">
         <v>8</v>
       </c>
-      <c r="L7" s="4"/>
-      <c r="N7" s="4">
+      <c r="L7" s="12"/>
+      <c r="N7" s="12">
         <v>0</v>
       </c>
-      <c r="O7" s="4"/>
+      <c r="O7" s="12"/>
     </row>
     <row r="8" spans="2:15">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="2">
         <f>COUNT(B5:B7)</f>
         <v>3</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="2">
         <f>COUNT(E5:E7)</f>
         <v>3</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="2">
         <f>COUNT(H5:H7)</f>
         <v>3</v>
       </c>
-      <c r="K8" s="10" t="s">
+      <c r="K8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L8" s="11">
+      <c r="L8" s="2">
         <f>COUNT(K5:K7)</f>
         <v>3</v>
       </c>
-      <c r="N8" s="10" t="s">
+      <c r="N8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="O8" s="11">
+      <c r="O8" s="2">
         <f>COUNT(N5:N7)</f>
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="2:15">
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="11">
+      <c r="C9" s="2">
         <f>SUM(B5:B7)</f>
         <v>8</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="2">
         <f>SUM(E5:E7)</f>
         <v>4</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I9" s="11">
+      <c r="I9" s="2">
         <f>SUM(H5:H7)</f>
         <v>18</v>
       </c>
-      <c r="K9" s="10" t="s">
+      <c r="K9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L9" s="11">
+      <c r="L9" s="2">
         <f>SUM(K5:K7)</f>
         <v>24</v>
       </c>
-      <c r="N9" s="10" t="s">
+      <c r="N9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O9" s="11">
+      <c r="O9" s="2">
         <f>SUM(N5:N7)</f>
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="2:15">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="2">
         <f>C9/C8</f>
         <v>2.6666666666666665</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="2">
         <f>F9/F8</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="2">
         <f>I9/I8</f>
         <v>6</v>
       </c>
-      <c r="K10" s="10" t="s">
+      <c r="K10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L10" s="11">
+      <c r="L10" s="2">
         <f>L9/L8</f>
         <v>8</v>
       </c>
-      <c r="N10" s="10" t="s">
+      <c r="N10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="O10" s="11">
+      <c r="O10" s="2">
         <f>O9/O8</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="2:15">
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="3">
         <f>ROUND(C10,0)</f>
         <v>3</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="3">
         <f>ROUND(F10,0)</f>
         <v>1</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="12">
+      <c r="I11" s="3">
         <f>ROUND(I10,0)</f>
         <v>6</v>
       </c>
-      <c r="K11" s="10" t="s">
+      <c r="K11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L11" s="12">
+      <c r="L11" s="3">
         <f>ROUND(L10,0)</f>
         <v>8</v>
       </c>
-      <c r="N11" s="10" t="s">
+      <c r="N11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O11" s="12">
+      <c r="O11" s="3">
         <f>ROUND(O10,0)</f>
         <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:15">
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="E13" s="3" t="s">
+      <c r="C13" s="13"/>
+      <c r="E13" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="3"/>
-      <c r="H13" s="3" t="s">
+      <c r="F13" s="13"/>
+      <c r="H13" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="I13" s="3"/>
-      <c r="K13" s="3" t="s">
+      <c r="I13" s="13"/>
+      <c r="K13" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="L13" s="3"/>
-      <c r="N13" s="3" t="s">
+      <c r="L13" s="13"/>
+      <c r="N13" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="O13" s="3"/>
+      <c r="O13" s="13"/>
     </row>
     <row r="14" spans="2:15">
-      <c r="B14" s="4">
+      <c r="B14" s="12">
         <v>6</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="E14" s="4">
+      <c r="C14" s="12"/>
+      <c r="E14" s="12">
         <v>4</v>
       </c>
-      <c r="F14" s="4"/>
-      <c r="H14" s="4">
+      <c r="F14" s="12"/>
+      <c r="H14" s="12">
         <v>6</v>
       </c>
-      <c r="I14" s="4"/>
-      <c r="K14" s="4">
+      <c r="I14" s="12"/>
+      <c r="K14" s="12">
         <v>10</v>
       </c>
-      <c r="L14" s="4"/>
-      <c r="N14" s="4">
+      <c r="L14" s="12"/>
+      <c r="N14" s="12">
         <v>0</v>
       </c>
-      <c r="O14" s="4"/>
+      <c r="O14" s="12"/>
     </row>
     <row r="15" spans="2:15">
-      <c r="B15" s="4">
+      <c r="B15" s="12">
         <v>0</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="E15" s="4">
+      <c r="C15" s="12"/>
+      <c r="E15" s="12">
         <v>6</v>
       </c>
-      <c r="F15" s="4"/>
-      <c r="H15" s="4">
+      <c r="F15" s="12"/>
+      <c r="H15" s="12">
         <v>5</v>
       </c>
-      <c r="I15" s="4"/>
-      <c r="K15" s="4">
+      <c r="I15" s="12"/>
+      <c r="K15" s="12">
         <v>8</v>
       </c>
-      <c r="L15" s="4"/>
-      <c r="N15" s="4">
+      <c r="L15" s="12"/>
+      <c r="N15" s="12">
         <v>8</v>
       </c>
-      <c r="O15" s="4"/>
+      <c r="O15" s="12"/>
     </row>
     <row r="16" spans="2:15">
-      <c r="B16" s="4">
+      <c r="B16" s="12">
         <v>4</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="E16" s="4">
+      <c r="C16" s="12"/>
+      <c r="E16" s="12">
         <v>5</v>
       </c>
-      <c r="F16" s="4"/>
-      <c r="H16" s="4">
+      <c r="F16" s="12"/>
+      <c r="H16" s="12">
         <v>4</v>
       </c>
-      <c r="I16" s="4"/>
-      <c r="K16" s="4">
+      <c r="I16" s="12"/>
+      <c r="K16" s="12">
         <v>10</v>
       </c>
-      <c r="L16" s="4"/>
-      <c r="N16" s="4">
+      <c r="L16" s="12"/>
+      <c r="N16" s="12">
         <v>7</v>
       </c>
-      <c r="O16" s="4"/>
+      <c r="O16" s="12"/>
     </row>
     <row r="17" spans="2:15">
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="2">
         <f>COUNT(B14:B16)</f>
         <v>3</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="2">
         <f>COUNT(E14:E16)</f>
         <v>3</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="H17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I17" s="11">
+      <c r="I17" s="2">
         <f>COUNT(H14:H16)</f>
         <v>3</v>
       </c>
-      <c r="K17" s="10" t="s">
+      <c r="K17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L17" s="11">
+      <c r="L17" s="2">
         <f>COUNT(K14:K16)</f>
         <v>3</v>
       </c>
-      <c r="N17" s="10" t="s">
+      <c r="N17" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="O17" s="11">
+      <c r="O17" s="2">
         <f>COUNT(N14:N16)</f>
         <v>3</v>
       </c>
     </row>
     <row r="18" spans="2:15">
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="2">
         <f>SUM(B14:B16)</f>
         <v>10</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="2">
         <f>SUM(E14:E16)</f>
         <v>15</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I18" s="11">
+      <c r="I18" s="2">
         <f>SUM(H14:H16)</f>
         <v>15</v>
       </c>
-      <c r="K18" s="10" t="s">
+      <c r="K18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L18" s="11">
+      <c r="L18" s="2">
         <f>SUM(K14:K16)</f>
         <v>28</v>
       </c>
-      <c r="N18" s="10" t="s">
+      <c r="N18" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O18" s="11">
+      <c r="O18" s="2">
         <f>SUM(N14:N16)</f>
         <v>15</v>
       </c>
     </row>
     <row r="19" spans="2:15">
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="11">
+      <c r="C19" s="2">
         <f>C18/C17</f>
         <v>3.3333333333333335</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="2">
         <f>F18/F17</f>
         <v>5</v>
       </c>
-      <c r="H19" s="10" t="s">
+      <c r="H19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I19" s="11">
+      <c r="I19" s="2">
         <f>I18/I17</f>
         <v>5</v>
       </c>
-      <c r="K19" s="10" t="s">
+      <c r="K19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L19" s="11">
+      <c r="L19" s="2">
         <f>L18/L17</f>
         <v>9.3333333333333339</v>
       </c>
-      <c r="N19" s="10" t="s">
+      <c r="N19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="O19" s="11">
+      <c r="O19" s="2">
         <f>O18/O17</f>
         <v>5</v>
       </c>
     </row>
     <row r="20" spans="2:15">
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C20" s="3">
         <f>ROUND(C19,0)</f>
         <v>3</v>
       </c>
-      <c r="E20" s="10" t="s">
+      <c r="E20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="12">
+      <c r="F20" s="3">
         <f>ROUND(F19,0)</f>
         <v>5</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I20" s="12">
+      <c r="I20" s="3">
         <f>ROUND(I19,0)</f>
         <v>5</v>
       </c>
-      <c r="K20" s="10" t="s">
+      <c r="K20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L20" s="12">
+      <c r="L20" s="3">
         <f>ROUND(L19,0)</f>
         <v>9</v>
       </c>
-      <c r="N20" s="10" t="s">
+      <c r="N20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O20" s="12">
+      <c r="O20" s="3">
         <f>ROUND(O19,0)</f>
         <v>5</v>
       </c>
@@ -3274,36 +3276,36 @@
       <c r="F22" s="8"/>
     </row>
     <row r="23" spans="2:15" ht="270" customHeight="1">
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D23" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E23" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F23" s="13" t="s">
+      <c r="F23" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="24" spans="2:15" ht="409.5">
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="13" t="s">
+      <c r="C24" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="13" t="s">
+      <c r="D24" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="E24" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F24" s="13" t="s">
+      <c r="F24" s="4" t="s">
         <v>22</v>
       </c>
     </row>
@@ -3366,417 +3368,417 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="30.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" style="14" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" style="14" customWidth="1"/>
-    <col min="4" max="4" width="34.7109375" style="14" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" style="14" customWidth="1"/>
-    <col min="6" max="6" width="34.5703125" style="14" customWidth="1"/>
-    <col min="7" max="1024" width="9.140625" style="14"/>
+    <col min="1" max="1" width="30.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="34.5703125" style="5" customWidth="1"/>
+    <col min="7" max="1024" width="9.140625" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:6" ht="18">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
     </row>
     <row r="3" spans="1:6" ht="15">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="5">
         <v>2</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="5">
         <v>3</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="5">
         <v>3</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="5">
         <v>0</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="5">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="5">
         <v>3.5</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="5">
         <v>3</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="5">
         <v>4</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="5">
         <v>2</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="5">
         <v>3.5</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="5">
         <v>3</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="5">
         <v>5</v>
       </c>
-      <c r="D6" s="14">
+      <c r="D6" s="5">
         <v>4</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="5">
         <v>2</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="5">
         <f>MIN(B4:B6)</f>
         <v>2</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="5">
         <f>MIN(C4:C6)</f>
         <v>3</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="5">
         <f>MIN(D4:D6)</f>
         <v>3</v>
       </c>
-      <c r="E9" s="14">
+      <c r="E9" s="5">
         <f>MIN(E4:E6)</f>
         <v>0</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="5">
         <f>MIN(F4:F6)</f>
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="5">
         <f>AVERAGE(B4:B6)</f>
         <v>2.8333333333333335</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="5">
         <f>AVERAGE(C4:C6)</f>
         <v>3.6666666666666665</v>
       </c>
-      <c r="D10" s="14">
+      <c r="D10" s="5">
         <f>AVERAGE(D4:D6)</f>
         <v>3.6666666666666665</v>
       </c>
-      <c r="E10" s="14">
+      <c r="E10" s="5">
         <f>AVERAGE(E4:E6)</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="F10" s="14">
+      <c r="F10" s="5">
         <f>AVERAGE(F4:F6)</f>
         <v>5.5</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="5">
         <f>MAX(B4:B6)</f>
         <v>3.5</v>
       </c>
-      <c r="C11" s="14">
+      <c r="C11" s="5">
         <f>MAX(C4:C6)</f>
         <v>5</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="5">
         <f>MAX(D4:D6)</f>
         <v>4</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="5">
         <f>MAX(E4:E6)</f>
         <v>2</v>
       </c>
-      <c r="F11" s="14">
+      <c r="F11" s="5">
         <f>MAX(F4:F6)</f>
         <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="17.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
     </row>
     <row r="14" spans="1:6" ht="15">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="14" t="s">
+      <c r="A15" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="14">
+      <c r="B15" s="5">
         <v>4</v>
       </c>
-      <c r="C15" s="14">
+      <c r="C15" s="5">
         <v>6</v>
       </c>
-      <c r="D15" s="14">
+      <c r="D15" s="5">
         <v>4</v>
       </c>
-      <c r="E15" s="14">
+      <c r="E15" s="5">
         <v>0</v>
       </c>
-      <c r="F15" s="14">
+      <c r="F15" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="14" t="s">
+      <c r="A16" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="14">
+      <c r="B16" s="5">
         <v>10</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C16" s="5">
         <v>4</v>
       </c>
-      <c r="D16" s="14">
+      <c r="D16" s="5">
         <v>5</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="5">
         <v>2</v>
       </c>
-      <c r="F16" s="14">
+      <c r="F16" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="14">
+      <c r="B17" s="5">
         <v>6</v>
       </c>
-      <c r="C17" s="14">
+      <c r="C17" s="5">
         <v>5</v>
       </c>
-      <c r="D17" s="14">
+      <c r="D17" s="5">
         <v>6</v>
       </c>
-      <c r="E17" s="14">
+      <c r="E17" s="5">
         <v>3</v>
       </c>
-      <c r="F17" s="14">
+      <c r="F17" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B18" s="5">
         <v>10</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C18" s="5">
         <v>8</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18" s="5">
         <v>8</v>
       </c>
-      <c r="E18" s="14">
+      <c r="E18" s="5">
         <v>10</v>
       </c>
-      <c r="F18" s="14">
+      <c r="F18" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="14">
+      <c r="B21" s="5">
         <f>MIN(B15:B18)</f>
         <v>4</v>
       </c>
-      <c r="C21" s="14">
+      <c r="C21" s="5">
         <f>MIN(C15:C18)</f>
         <v>4</v>
       </c>
-      <c r="D21" s="14">
+      <c r="D21" s="5">
         <f>MIN(D15:D18)</f>
         <v>4</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E21" s="5">
         <f>MIN(E15:E18)</f>
         <v>0</v>
       </c>
-      <c r="F21" s="14">
+      <c r="F21" s="5">
         <f>MIN(F15:F18)</f>
         <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="14" t="s">
+      <c r="A22" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="14">
+      <c r="B22" s="5">
         <f>AVERAGE(B15:B18)</f>
         <v>7.5</v>
       </c>
-      <c r="C22" s="14">
+      <c r="C22" s="5">
         <f>AVERAGE(C15:C18)</f>
         <v>5.75</v>
       </c>
-      <c r="D22" s="14">
+      <c r="D22" s="5">
         <f>AVERAGE(D15:D18)</f>
         <v>5.75</v>
       </c>
-      <c r="E22" s="14">
+      <c r="E22" s="5">
         <f>AVERAGE(E15:E18)</f>
         <v>3.75</v>
       </c>
-      <c r="F22" s="14">
+      <c r="F22" s="5">
         <f>AVERAGE(F15:F18)</f>
         <v>9</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="14">
+      <c r="B23" s="5">
         <f>MAX(B15:B18)</f>
         <v>10</v>
       </c>
-      <c r="C23" s="14">
+      <c r="C23" s="5">
         <f>MAX(C15:C18)</f>
         <v>8</v>
       </c>
-      <c r="D23" s="14">
+      <c r="D23" s="5">
         <f>MAX(D15:D18)</f>
         <v>8</v>
       </c>
-      <c r="E23" s="14">
+      <c r="E23" s="5">
         <f>MAX(E15:E18)</f>
         <v>10</v>
       </c>
-      <c r="F23" s="14">
+      <c r="F23" s="5">
         <f>MAX(F15:F18)</f>
         <v>10</v>
       </c>
@@ -3794,399 +3796,399 @@
     </row>
     <row r="26" spans="1:6" ht="15"/>
     <row r="27" spans="1:6">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="14">
+      <c r="B28" s="5">
         <f>B22</f>
         <v>7.5</v>
       </c>
-      <c r="C28" s="14">
+      <c r="C28" s="5">
         <f>B10</f>
         <v>2.8333333333333335</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="14">
+      <c r="B29" s="5">
         <f>C22</f>
         <v>5.75</v>
       </c>
-      <c r="C29" s="14">
+      <c r="C29" s="5">
         <f>C10</f>
         <v>3.6666666666666665</v>
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B30" s="14">
+      <c r="B30" s="5">
         <f>D22</f>
         <v>5.75</v>
       </c>
-      <c r="C30" s="14">
+      <c r="C30" s="5">
         <f>D10</f>
         <v>3.6666666666666665</v>
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B31" s="14">
+      <c r="B31" s="5">
         <f>E22</f>
         <v>3.75</v>
       </c>
-      <c r="C31" s="14">
+      <c r="C31" s="5">
         <f>E10</f>
         <v>1.3333333333333333</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="14">
+      <c r="B32" s="5">
         <f>F22</f>
         <v>9</v>
       </c>
-      <c r="C32" s="14">
+      <c r="C32" s="5">
         <f>F10</f>
         <v>5.5</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15"/>
     <row r="34" spans="1:6" ht="19.5">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
     </row>
     <row r="35" spans="1:6" ht="16.5">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
+      <c r="B35" s="14"/>
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
     </row>
     <row r="36" spans="1:6" ht="15">
-      <c r="A36" s="14" t="s">
+      <c r="A36" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C36" s="15" t="s">
+      <c r="C36" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D36" s="15" t="s">
+      <c r="D36" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E36" s="15" t="s">
+      <c r="E36" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F36" s="15" t="s">
+      <c r="F36" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="14">
+      <c r="B37" s="5">
         <f>MIN(B4:B6)</f>
         <v>2</v>
       </c>
-      <c r="C37" s="14">
+      <c r="C37" s="5">
         <f>MIN(C4:C6)</f>
         <v>3</v>
       </c>
-      <c r="D37" s="14">
+      <c r="D37" s="5">
         <f>MIN(D4:D6)</f>
         <v>3</v>
       </c>
-      <c r="E37" s="14">
+      <c r="E37" s="5">
         <f>MIN(E4:E6)</f>
         <v>0</v>
       </c>
-      <c r="F37" s="14">
+      <c r="F37" s="5">
         <f>MIN(F4:F6)</f>
         <v>3</v>
       </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="14" t="s">
+      <c r="A38" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="14">
+      <c r="B38" s="5">
         <f>QUARTILE(B4:B6,1)</f>
         <v>2.5</v>
       </c>
-      <c r="C38" s="14">
+      <c r="C38" s="5">
         <f>QUARTILE(C4:C6,1)</f>
         <v>3</v>
       </c>
-      <c r="D38" s="14">
+      <c r="D38" s="5">
         <f>QUARTILE(D4:D6,1)</f>
         <v>3.5</v>
       </c>
-      <c r="E38" s="14">
+      <c r="E38" s="5">
         <f>QUARTILE(E4:E6,1)</f>
         <v>1</v>
       </c>
-      <c r="F38" s="14">
+      <c r="F38" s="5">
         <f>QUARTILE(F4:F6,1)</f>
         <v>3.25</v>
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="14" t="s">
+      <c r="A39" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B39" s="14">
+      <c r="B39" s="5">
         <f>QUARTILE(B4:B6,2)</f>
         <v>3</v>
       </c>
-      <c r="C39" s="14">
+      <c r="C39" s="5">
         <f>QUARTILE(C4:C6,2)</f>
         <v>3</v>
       </c>
-      <c r="D39" s="14">
+      <c r="D39" s="5">
         <f>QUARTILE(D4:D6,2)</f>
         <v>4</v>
       </c>
-      <c r="E39" s="14">
+      <c r="E39" s="5">
         <f>QUARTILE(E4:E6,2)</f>
         <v>2</v>
       </c>
-      <c r="F39" s="14">
+      <c r="F39" s="5">
         <f>QUARTILE(F4:F6,2)</f>
         <v>3.5</v>
       </c>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="14" t="s">
+      <c r="A40" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B40" s="14">
+      <c r="B40" s="5">
         <f>QUARTILE(B4:B6,3)</f>
         <v>3.25</v>
       </c>
-      <c r="C40" s="14">
+      <c r="C40" s="5">
         <f>QUARTILE(C4:C6,3)</f>
         <v>4</v>
       </c>
-      <c r="D40" s="14">
+      <c r="D40" s="5">
         <f>QUARTILE(D4:D6,3)</f>
         <v>4</v>
       </c>
-      <c r="E40" s="14">
+      <c r="E40" s="5">
         <f>QUARTILE(E4:E6,3)</f>
         <v>2</v>
       </c>
-      <c r="F40" s="14">
+      <c r="F40" s="5">
         <f>QUARTILE(F4:F6,3)</f>
         <v>6.75</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="15">
-      <c r="A41" s="14" t="s">
+      <c r="A41" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B41" s="14">
+      <c r="B41" s="5">
         <f>MAX(B4:B6)</f>
         <v>3.5</v>
       </c>
-      <c r="C41" s="14">
+      <c r="C41" s="5">
         <f>MAX(C6)</f>
         <v>5</v>
       </c>
-      <c r="D41" s="14">
+      <c r="D41" s="5">
         <f>MAX(D4:D6)</f>
         <v>4</v>
       </c>
-      <c r="E41" s="14">
+      <c r="E41" s="5">
         <f>MAX(E4:E6)</f>
         <v>2</v>
       </c>
-      <c r="F41" s="14">
+      <c r="F41" s="5">
         <f>MAX(F4:F6)</f>
         <v>10</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="15"/>
     <row r="43" spans="1:6" ht="16.5">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
     </row>
     <row r="44" spans="1:6" ht="15">
-      <c r="A44" s="14" t="s">
+      <c r="A44" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C44" s="15" t="s">
+      <c r="C44" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D44" s="15" t="s">
+      <c r="D44" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E44" s="15" t="s">
+      <c r="E44" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F44" s="15" t="s">
+      <c r="F44" s="6" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="14" t="s">
+      <c r="A45" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B45" s="14">
+      <c r="B45" s="5">
         <f>MIN(B15:B18)</f>
         <v>4</v>
       </c>
-      <c r="C45" s="14">
+      <c r="C45" s="5">
         <f>MIN(C15:C18)</f>
         <v>4</v>
       </c>
-      <c r="D45" s="14">
+      <c r="D45" s="5">
         <f>MIN(D15:D18)</f>
         <v>4</v>
       </c>
-      <c r="E45" s="14">
+      <c r="E45" s="5">
         <f>MIN(E15:E18)</f>
         <v>0</v>
       </c>
-      <c r="F45" s="14">
+      <c r="F45" s="5">
         <f>MIN(F15:F18)</f>
         <v>6</v>
       </c>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" s="14" t="s">
+      <c r="A46" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="14">
+      <c r="B46" s="5">
         <f>QUARTILE(B15:B18,1)</f>
         <v>5.5</v>
       </c>
-      <c r="C46" s="14">
+      <c r="C46" s="5">
         <f>QUARTILE(C15:C18,1)</f>
         <v>4.75</v>
       </c>
-      <c r="D46" s="14">
+      <c r="D46" s="5">
         <f>QUARTILE(D15:D18,1)</f>
         <v>4.75</v>
       </c>
-      <c r="E46" s="14">
+      <c r="E46" s="5">
         <f>QUARTILE(E15:E18,1)</f>
         <v>1.5</v>
       </c>
-      <c r="F46" s="14">
+      <c r="F46" s="5">
         <f>QUARTILE(F15:F18,1)</f>
         <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" s="14" t="s">
+      <c r="A47" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B47" s="14">
+      <c r="B47" s="5">
         <f>QUARTILE(B15:B18,2)</f>
         <v>8</v>
       </c>
-      <c r="C47" s="14">
+      <c r="C47" s="5">
         <f>QUARTILE(C15:C18,2)</f>
         <v>5.5</v>
       </c>
-      <c r="D47" s="14">
+      <c r="D47" s="5">
         <f>QUARTILE(D15:D18,2)</f>
         <v>5.5</v>
       </c>
-      <c r="E47" s="14">
+      <c r="E47" s="5">
         <f>QUARTILE(E15:E18,2)</f>
         <v>2.5</v>
       </c>
-      <c r="F47" s="14">
+      <c r="F47" s="5">
         <f>QUARTILE(F15:F18,2)</f>
         <v>10</v>
       </c>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="14" t="s">
+      <c r="A48" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="14">
+      <c r="B48" s="5">
         <f>QUARTILE(B15:B18,3)</f>
         <v>10</v>
       </c>
-      <c r="C48" s="14">
+      <c r="C48" s="5">
         <f>QUARTILE(C15:C18,3)</f>
         <v>6.5</v>
       </c>
-      <c r="D48" s="14">
+      <c r="D48" s="5">
         <f>QUARTILE(D15:D18,3)</f>
         <v>6.5</v>
       </c>
-      <c r="E48" s="14">
+      <c r="E48" s="5">
         <f>QUARTILE(E15:E18,3)</f>
         <v>4.75</v>
       </c>
-      <c r="F48" s="14">
+      <c r="F48" s="5">
         <f>QUARTILE(F15:F18,3)</f>
         <v>10</v>
       </c>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="14" t="s">
+      <c r="A49" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B49" s="14">
+      <c r="B49" s="5">
         <f>MAX(B15:B18)</f>
         <v>10</v>
       </c>
-      <c r="C49" s="14">
+      <c r="C49" s="5">
         <f>MAX(C15:C18)</f>
         <v>8</v>
       </c>
-      <c r="D49" s="14">
+      <c r="D49" s="5">
         <f>MAX(D15:D18)</f>
         <v>8</v>
       </c>
-      <c r="E49" s="14">
+      <c r="E49" s="5">
         <f>MAX(E15:E18)</f>
         <v>10</v>
       </c>
-      <c r="F49" s="14">
+      <c r="F49" s="5">
         <f>MAX(F15:F18)</f>
         <v>10</v>
       </c>

</xml_diff>